<commit_message>
Made seasonality more logical
</commit_message>
<xml_diff>
--- a/data/Data.xlsx
+++ b/data/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\Projects\Python Projects\DemandPredictor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\Projects\Python Projects\DemandPredictor\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7AD32C-D943-488E-85F8-7837919A67A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E29E50-605A-4FED-97C7-433F32B77C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,7 +1056,7 @@
         <v>91</v>
       </c>
       <c r="P13">
-        <v>1700</v>
+        <v>1720</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">

</xml_diff>